<commit_message>
Added Color To Positions in editor
</commit_message>
<xml_diff>
--- a/DiseñoDePruebas.xlsx
+++ b/DiseñoDePruebas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>El valor de un equipo refleja la suma de todos los jugadores si los titulares son validos.</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>Al terminarse un torneo, se mostraran los 3 mejores jugadores cuyo equipo sea valido.</t>
+  </si>
+  <si>
+    <t>Prueba</t>
+  </si>
+  <si>
+    <t>Resultado</t>
   </si>
 </sst>
 </file>
@@ -374,58 +380,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:B12"/>
+  <dimension ref="B1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="103" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deleted 2 Unused Classes
</commit_message>
<xml_diff>
--- a/DiseñoDePruebas.xlsx
+++ b/DiseñoDePruebas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
   <si>
     <t>El valor de un equipo refleja la suma de todos los jugadores si los titulares son validos.</t>
   </si>
@@ -57,13 +57,16 @@
   </si>
   <si>
     <t>Si</t>
+  </si>
+  <si>
+    <t>Resultado Esperado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,13 +82,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -97,14 +112,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -383,90 +401,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:F12"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="103" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="103" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
       <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>